<commit_message>
Penambahan Report Hasil Tindak Lanjut
</commit_message>
<xml_diff>
--- a/vendor/template/template_laporan.xlsx
+++ b/vendor/template/template_laporan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\DashboardTPB\vendor\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA38968-66C1-44F6-A3ED-2EB8CFBDA960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DDE020-3729-45D6-BB5A-0BA8A14A2F6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Worksheet!$A:$H</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Worksheet!$A$1:$I$14</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Worksheet!$13:$13</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>NPWP</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>TINDAK LANJUT</t>
+  </si>
+  <si>
+    <t>HASIL TINDAK LANJUT</t>
   </si>
 </sst>
 </file>
@@ -172,11 +175,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,126 +488,137 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:H11"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="25" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="25" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="2.85546875" style="2"/>
+    <col min="8" max="8" width="22.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="2.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
@@ -629,8 +643,11 @@
       <c r="H13" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" ht="2.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="3" customFormat="1" ht="2.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -642,10 +659,10 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="2">
-    <mergeCell ref="B1:H8"/>
-    <mergeCell ref="A10:H11"/>
+    <mergeCell ref="B1:I8"/>
+    <mergeCell ref="A10:I11"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.94488188976377963" top="0" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>